<commit_message>
Actualización del archivo de APN's
</commit_message>
<xml_diff>
--- a/Standard/APN'S.xlsx
+++ b/Standard/APN'S.xlsx
@@ -8,8 +8,6 @@
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
-    <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
@@ -126,10 +124,10 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -447,16 +445,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="5"/>
+      <c r="B1" s="6"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="6"/>
+      <c r="B3" s="5"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
@@ -479,10 +477,10 @@
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="6"/>
+      <c r="B8" s="5"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
@@ -505,10 +503,10 @@
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="6"/>
+      <c r="B13" s="5"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
@@ -540,28 +538,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>